<commit_message>
updated plots and edited readme
</commit_message>
<xml_diff>
--- a/hand_sieved_data_modified.xlsx
+++ b/hand_sieved_data_modified.xlsx
@@ -146,9 +146,6 @@
     <t xml:space="preserve">0.625-0.125 </t>
   </si>
   <si>
-    <t xml:space="preserve">&gt; 2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">0.500-1 </t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.0625- 0.125 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;2 </t>
   </si>
 </sst>
 </file>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="I157" sqref="I157"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -567,7 +567,7 @@
         <v>99.11</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>2.1511999999999998</v>
@@ -766,7 +766,7 @@
         <v>111.67</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E9">
         <v>2.1981999999999999</v>
@@ -935,7 +935,7 @@
         <v>98.65</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E16">
         <v>2.1758999999999999</v>
@@ -1103,7 +1103,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E23">
         <v>2.2229999999999999</v>
@@ -1112,7 +1112,7 @@
         <v>2.5274000000000001</v>
       </c>
       <c r="G23">
-        <f>F23-E23</f>
+        <f t="shared" ref="G23:G43" si="3">F23-E23</f>
         <v>0.30440000000000023</v>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
         <v>2.375</v>
       </c>
       <c r="G24">
-        <f>F24-E24</f>
+        <f t="shared" si="3"/>
         <v>0.15289999999999981</v>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25">
         <v>2.2052999999999998</v>
@@ -1160,7 +1160,7 @@
         <v>2.3592</v>
       </c>
       <c r="G25">
-        <f>F25-E25</f>
+        <f t="shared" si="3"/>
         <v>0.15390000000000015</v>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26">
         <v>2.2170999999999998</v>
@@ -1184,7 +1184,7 @@
         <v>2.3675000000000002</v>
       </c>
       <c r="G26">
-        <f>F26-E26</f>
+        <f t="shared" si="3"/>
         <v>0.15040000000000031</v>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27">
         <v>2.2166999999999999</v>
@@ -1208,7 +1208,7 @@
         <v>3.3441999999999998</v>
       </c>
       <c r="G27">
-        <f>F27-E27</f>
+        <f t="shared" si="3"/>
         <v>1.1274999999999999</v>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28">
         <v>2.2299000000000002</v>
@@ -1232,7 +1232,7 @@
         <v>14.279199999999999</v>
       </c>
       <c r="G28">
-        <f>F28-E28</f>
+        <f t="shared" si="3"/>
         <v>12.049299999999999</v>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
         <v>18.309999999999999</v>
       </c>
       <c r="G29">
-        <f>F29-E29</f>
+        <f t="shared" si="3"/>
         <v>6.1899999999999995</v>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E30">
         <v>2.2029999999999998</v>
@@ -1280,7 +1280,7 @@
         <v>2.3338000000000001</v>
       </c>
       <c r="G30">
-        <f>F30-E30</f>
+        <f t="shared" si="3"/>
         <v>0.13080000000000025</v>
       </c>
     </row>
@@ -1304,7 +1304,7 @@
         <v>2.3959999999999999</v>
       </c>
       <c r="G31">
-        <f>F31-E31</f>
+        <f t="shared" si="3"/>
         <v>0.17879999999999985</v>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32">
         <v>2.1997</v>
@@ -1328,7 +1328,7 @@
         <v>2.3469000000000002</v>
       </c>
       <c r="G32">
-        <f>F32-E32</f>
+        <f t="shared" si="3"/>
         <v>0.14720000000000022</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33">
         <v>2.2065000000000001</v>
@@ -1352,7 +1352,7 @@
         <v>2.3805999999999998</v>
       </c>
       <c r="G33">
-        <f>F33-E33</f>
+        <f t="shared" si="3"/>
         <v>0.1740999999999997</v>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34">
         <v>2.2016</v>
@@ -1376,7 +1376,7 @@
         <v>3.3206000000000002</v>
       </c>
       <c r="G34">
-        <f>F34-E34</f>
+        <f t="shared" si="3"/>
         <v>1.1190000000000002</v>
       </c>
       <c r="P34" s="12"/>
@@ -1400,7 +1400,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E35">
         <v>2.2225999999999999</v>
@@ -1409,7 +1409,7 @@
         <v>13.8889</v>
       </c>
       <c r="G35">
-        <f>F35-E35</f>
+        <f t="shared" si="3"/>
         <v>11.6663</v>
       </c>
     </row>
@@ -1433,7 +1433,7 @@
         <v>18.98</v>
       </c>
       <c r="G36">
-        <f>F36-E36</f>
+        <f t="shared" si="3"/>
         <v>6.93</v>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
         <v>49.9739</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E37">
         <v>2.2119</v>
@@ -1457,7 +1457,7 @@
         <v>3.3849999999999998</v>
       </c>
       <c r="G37">
-        <f>F37-E37</f>
+        <f t="shared" si="3"/>
         <v>1.1730999999999998</v>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
         <v>2.3927999999999998</v>
       </c>
       <c r="G38">
-        <f>F38-E38</f>
+        <f t="shared" si="3"/>
         <v>0.17749999999999977</v>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
         <v>49.9739</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39">
         <v>2.2149999999999999</v>
@@ -1505,7 +1505,7 @@
         <v>2.3490000000000002</v>
       </c>
       <c r="G39">
-        <f>F39-E39</f>
+        <f t="shared" si="3"/>
         <v>0.13400000000000034</v>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
         <v>49.9739</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40">
         <v>2.2242000000000002</v>
@@ -1529,7 +1529,7 @@
         <v>2.5215999999999998</v>
       </c>
       <c r="G40">
-        <f>F40-E40</f>
+        <f t="shared" si="3"/>
         <v>0.29739999999999966</v>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
         <v>49.9739</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41">
         <v>2.2006000000000001</v>
@@ -1553,7 +1553,7 @@
         <v>3.6427999999999998</v>
       </c>
       <c r="G41">
-        <f>F41-E41</f>
+        <f t="shared" si="3"/>
         <v>1.4421999999999997</v>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
         <v>49.9739</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E42">
         <v>2.2153</v>
@@ -1577,7 +1577,7 @@
         <v>15.960800000000001</v>
       </c>
       <c r="G42">
-        <f>F42-E42</f>
+        <f t="shared" si="3"/>
         <v>13.7455</v>
       </c>
     </row>
@@ -1601,7 +1601,7 @@
         <v>16.260000000000002</v>
       </c>
       <c r="G43">
-        <f>F43-E43</f>
+        <f t="shared" si="3"/>
         <v>4.2600000000000016</v>
       </c>
     </row>
@@ -1616,7 +1616,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E44">
         <v>2.2229999999999999</v>
@@ -1625,7 +1625,7 @@
         <v>2.5274000000000001</v>
       </c>
       <c r="G44">
-        <f t="shared" ref="G44:G64" si="3">F44-E44</f>
+        <f t="shared" ref="G44:G64" si="4">F44-E44</f>
         <v>0.30440000000000023</v>
       </c>
     </row>
@@ -1649,7 +1649,7 @@
         <v>2.375</v>
       </c>
       <c r="G45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15289999999999981</v>
       </c>
     </row>
@@ -1664,7 +1664,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46">
         <v>2.2052999999999998</v>
@@ -1673,7 +1673,7 @@
         <v>2.3592</v>
       </c>
       <c r="G46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15390000000000015</v>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E47">
         <v>2.2170999999999998</v>
@@ -1697,7 +1697,7 @@
         <v>2.3675000000000002</v>
       </c>
       <c r="G47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15040000000000031</v>
       </c>
     </row>
@@ -1712,7 +1712,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48">
         <v>2.2166999999999999</v>
@@ -1721,7 +1721,7 @@
         <v>3.3441999999999998</v>
       </c>
       <c r="G48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1274999999999999</v>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
         <v>50.152999999999999</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49">
         <v>2.2299000000000002</v>
@@ -1745,7 +1745,7 @@
         <v>14.279199999999999</v>
       </c>
       <c r="G49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.049299999999999</v>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
         <v>18.309999999999999</v>
       </c>
       <c r="G50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.1899999999999995</v>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E51">
         <v>2.2029999999999998</v>
@@ -1793,7 +1793,7 @@
         <v>2.3338000000000001</v>
       </c>
       <c r="G51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13080000000000025</v>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
         <v>2.3959999999999999</v>
       </c>
       <c r="G52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17879999999999985</v>
       </c>
     </row>
@@ -1832,7 +1832,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E53">
         <v>2.1997</v>
@@ -1841,7 +1841,7 @@
         <v>2.3469000000000002</v>
       </c>
       <c r="G53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.14720000000000022</v>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E54">
         <v>2.2065000000000001</v>
@@ -1865,7 +1865,7 @@
         <v>2.3805999999999998</v>
       </c>
       <c r="G54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1740999999999997</v>
       </c>
     </row>
@@ -1880,7 +1880,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E55">
         <v>2.2016</v>
@@ -1889,7 +1889,7 @@
         <v>3.3206000000000002</v>
       </c>
       <c r="G55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1190000000000002</v>
       </c>
     </row>
@@ -1904,7 +1904,7 @@
         <v>50.214300000000001</v>
       </c>
       <c r="D56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E56">
         <v>2.2225999999999999</v>
@@ -1913,7 +1913,7 @@
         <v>13.8889</v>
       </c>
       <c r="G56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.6663</v>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
         <v>18.98</v>
       </c>
       <c r="G57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.93</v>
       </c>
     </row>
@@ -1952,7 +1952,7 @@
         <v>49.9739</v>
       </c>
       <c r="D58" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E58">
         <v>2.2119</v>
@@ -1961,7 +1961,7 @@
         <v>3.3849999999999998</v>
       </c>
       <c r="G58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1730999999999998</v>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
         <v>2.3927999999999998</v>
       </c>
       <c r="G59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17749999999999977</v>
       </c>
     </row>
@@ -2000,7 +2000,7 @@
         <v>49.9739</v>
       </c>
       <c r="D60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E60">
         <v>2.2149999999999999</v>
@@ -2009,7 +2009,7 @@
         <v>2.3490000000000002</v>
       </c>
       <c r="G60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13400000000000034</v>
       </c>
     </row>
@@ -2024,7 +2024,7 @@
         <v>49.9739</v>
       </c>
       <c r="D61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E61">
         <v>2.2242000000000002</v>
@@ -2033,7 +2033,7 @@
         <v>2.5215999999999998</v>
       </c>
       <c r="G61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29739999999999966</v>
       </c>
     </row>
@@ -2048,7 +2048,7 @@
         <v>49.9739</v>
       </c>
       <c r="D62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E62">
         <v>2.2006000000000001</v>
@@ -2057,7 +2057,7 @@
         <v>3.6427999999999998</v>
       </c>
       <c r="G62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4421999999999997</v>
       </c>
     </row>
@@ -2072,7 +2072,7 @@
         <v>49.9739</v>
       </c>
       <c r="D63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E63">
         <v>2.2153</v>
@@ -2081,7 +2081,7 @@
         <v>15.960800000000001</v>
       </c>
       <c r="G63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.7455</v>
       </c>
     </row>
@@ -2105,7 +2105,7 @@
         <v>16.260000000000002</v>
       </c>
       <c r="G64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2600000000000016</v>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
         <v>50.08</v>
       </c>
       <c r="D65" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E65">
         <v>2.2271999999999998</v>
@@ -2129,7 +2129,7 @@
         <v>2.7585999999999999</v>
       </c>
       <c r="G65">
-        <f t="shared" ref="G65:G75" si="4">F65-E65</f>
+        <f t="shared" ref="G65:G75" si="5">F65-E65</f>
         <v>0.53140000000000009</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
         <v>9.9289000000000005</v>
       </c>
       <c r="G66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.7292000000000005</v>
       </c>
     </row>
@@ -2168,7 +2168,7 @@
         <v>50.08</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E67">
         <v>2.1966999999999999</v>
@@ -2177,7 +2177,7 @@
         <v>31.273700000000002</v>
       </c>
       <c r="G67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.077000000000002</v>
       </c>
     </row>
@@ -2192,7 +2192,7 @@
         <v>50.08</v>
       </c>
       <c r="D68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E68">
         <v>2.2530000000000001</v>
@@ -2201,7 +2201,7 @@
         <v>7.5494000000000003</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.2964000000000002</v>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
         <v>50.08</v>
       </c>
       <c r="D69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E69">
         <v>2.1907000000000001</v>
@@ -2225,7 +2225,7 @@
         <v>3.2311000000000001</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0404</v>
       </c>
     </row>
@@ -2240,7 +2240,7 @@
         <v>50.08</v>
       </c>
       <c r="D70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E70">
         <v>2.3243999999999998</v>
@@ -2249,7 +2249,7 @@
         <v>2.5724</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.24800000000000022</v>
       </c>
     </row>
@@ -2273,7 +2273,7 @@
         <v>14.4</v>
       </c>
       <c r="G71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.34</v>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
         <v>50.03</v>
       </c>
       <c r="D72" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E72">
         <v>2.2406999999999999</v>
@@ -2297,7 +2297,7 @@
         <v>3.1456</v>
       </c>
       <c r="G72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.90490000000000004</v>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
         <v>11.8307</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5957000000000008</v>
       </c>
     </row>
@@ -2336,7 +2336,7 @@
         <v>50.03</v>
       </c>
       <c r="D74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E74">
         <v>2.2010000000000001</v>
@@ -2345,7 +2345,7 @@
         <v>29.123699999999999</v>
       </c>
       <c r="G74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.922699999999999</v>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
         <v>50.03</v>
       </c>
       <c r="D75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E75">
         <v>2.2557999999999998</v>
@@ -2369,7 +2369,7 @@
         <v>7.2332999999999998</v>
       </c>
       <c r="G75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9775</v>
       </c>
     </row>
@@ -2384,7 +2384,7 @@
         <v>50.03</v>
       </c>
       <c r="D76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E76">
         <v>2.2364999999999999</v>
@@ -2393,7 +2393,7 @@
         <v>2.8180000000000001</v>
       </c>
       <c r="G76">
-        <f>F76-E76</f>
+        <f t="shared" ref="G76:G109" si="6">F76-E76</f>
         <v>0.58150000000000013</v>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
         <v>50.03</v>
       </c>
       <c r="D77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E77">
         <v>2.2368000000000001</v>
@@ -2417,7 +2417,7 @@
         <v>2.4218000000000002</v>
       </c>
       <c r="G77">
-        <f>F77-E77</f>
+        <f t="shared" si="6"/>
         <v>0.18500000000000005</v>
       </c>
     </row>
@@ -2441,7 +2441,7 @@
         <v>15.76</v>
       </c>
       <c r="G78">
-        <f>F78-E78</f>
+        <f t="shared" si="6"/>
         <v>3.7099999999999991</v>
       </c>
       <c r="H78" s="2"/>
@@ -2457,7 +2457,7 @@
         <v>50.05</v>
       </c>
       <c r="D79" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E79">
         <v>1.2595000000000001</v>
@@ -2466,7 +2466,7 @@
         <v>1.8945000000000001</v>
       </c>
       <c r="G79">
-        <f>F79-E79</f>
+        <f t="shared" si="6"/>
         <v>0.63500000000000001</v>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
         <v>10.7417</v>
       </c>
       <c r="G80">
-        <f>F80-E80</f>
+        <f t="shared" si="6"/>
         <v>9.4780999999999995</v>
       </c>
       <c r="R80" s="7"/>
@@ -2507,7 +2507,7 @@
         <v>50.05</v>
       </c>
       <c r="D81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E81">
         <v>2.1850999999999998</v>
@@ -2516,7 +2516,7 @@
         <v>27.6266</v>
       </c>
       <c r="G81">
-        <f>F81-E81</f>
+        <f t="shared" si="6"/>
         <v>25.441500000000001</v>
       </c>
       <c r="R81" s="7"/>
@@ -2533,7 +2533,7 @@
         <v>50.05</v>
       </c>
       <c r="D82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E82">
         <v>2.1972999999999998</v>
@@ -2542,7 +2542,7 @@
         <v>11.6435</v>
       </c>
       <c r="G82">
-        <f>F82-E82</f>
+        <f t="shared" si="6"/>
         <v>9.4461999999999993</v>
       </c>
       <c r="R82" s="7"/>
@@ -2559,7 +2559,7 @@
         <v>50.05</v>
       </c>
       <c r="D83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E83">
         <v>2.2465999999999999</v>
@@ -2568,7 +2568,7 @@
         <v>2.5966999999999998</v>
       </c>
       <c r="G83">
-        <f>F83-E83</f>
+        <f t="shared" si="6"/>
         <v>0.35009999999999986</v>
       </c>
       <c r="R83" s="7"/>
@@ -2585,7 +2585,7 @@
         <v>50.05</v>
       </c>
       <c r="D84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E84">
         <v>1.2765</v>
@@ -2594,7 +2594,7 @@
         <v>1.6495</v>
       </c>
       <c r="G84">
-        <f>F84-E84</f>
+        <f t="shared" si="6"/>
         <v>0.373</v>
       </c>
       <c r="R84" s="7"/>
@@ -2620,7 +2620,7 @@
         <v>15.92</v>
       </c>
       <c r="G85">
-        <f>F85-E85</f>
+        <f t="shared" si="6"/>
         <v>3.7899999999999991</v>
       </c>
       <c r="R85" s="7"/>
@@ -2637,7 +2637,7 @@
         <v>50.08</v>
       </c>
       <c r="D86" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E86">
         <v>2.2271999999999998</v>
@@ -2646,7 +2646,7 @@
         <v>2.7585999999999999</v>
       </c>
       <c r="G86">
-        <f>F86-E86</f>
+        <f t="shared" si="6"/>
         <v>0.53140000000000009</v>
       </c>
       <c r="R86" s="7"/>
@@ -2672,7 +2672,7 @@
         <v>9.9289000000000005</v>
       </c>
       <c r="G87">
-        <f>F87-E87</f>
+        <f t="shared" si="6"/>
         <v>7.7292000000000005</v>
       </c>
       <c r="R87" s="7"/>
@@ -2689,7 +2689,7 @@
         <v>50.08</v>
       </c>
       <c r="D88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E88">
         <v>2.1966999999999999</v>
@@ -2698,7 +2698,7 @@
         <v>31.273700000000002</v>
       </c>
       <c r="G88">
-        <f>F88-E88</f>
+        <f t="shared" si="6"/>
         <v>29.077000000000002</v>
       </c>
       <c r="R88" s="7"/>
@@ -2715,7 +2715,7 @@
         <v>50.08</v>
       </c>
       <c r="D89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E89">
         <v>2.2530000000000001</v>
@@ -2724,7 +2724,7 @@
         <v>7.5494000000000003</v>
       </c>
       <c r="G89">
-        <f>F89-E89</f>
+        <f t="shared" si="6"/>
         <v>5.2964000000000002</v>
       </c>
       <c r="P89" s="7"/>
@@ -2743,7 +2743,7 @@
         <v>50.08</v>
       </c>
       <c r="D90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E90">
         <v>2.1907000000000001</v>
@@ -2752,7 +2752,7 @@
         <v>3.2311000000000001</v>
       </c>
       <c r="G90">
-        <f>F90-E90</f>
+        <f t="shared" si="6"/>
         <v>1.0404</v>
       </c>
       <c r="P90" s="13"/>
@@ -2771,7 +2771,7 @@
         <v>50.08</v>
       </c>
       <c r="D91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E91">
         <v>2.3243999999999998</v>
@@ -2780,7 +2780,7 @@
         <v>2.5724</v>
       </c>
       <c r="G91">
-        <f>F91-E91</f>
+        <f t="shared" si="6"/>
         <v>0.24800000000000022</v>
       </c>
       <c r="P91" s="7"/>
@@ -2808,7 +2808,7 @@
         <v>14.4</v>
       </c>
       <c r="G92">
-        <f>F92-E92</f>
+        <f t="shared" si="6"/>
         <v>2.34</v>
       </c>
       <c r="H92"/>
@@ -2828,7 +2828,7 @@
         <v>50.03</v>
       </c>
       <c r="D93" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E93">
         <v>2.2406999999999999</v>
@@ -2837,7 +2837,7 @@
         <v>3.1456</v>
       </c>
       <c r="G93">
-        <f>F93-E93</f>
+        <f t="shared" si="6"/>
         <v>0.90490000000000004</v>
       </c>
     </row>
@@ -2861,7 +2861,7 @@
         <v>11.8307</v>
       </c>
       <c r="G94">
-        <f>F94-E94</f>
+        <f t="shared" si="6"/>
         <v>9.5957000000000008</v>
       </c>
     </row>
@@ -2876,7 +2876,7 @@
         <v>50.03</v>
       </c>
       <c r="D95" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E95">
         <v>2.2010000000000001</v>
@@ -2885,7 +2885,7 @@
         <v>29.123699999999999</v>
       </c>
       <c r="G95">
-        <f>F95-E95</f>
+        <f t="shared" si="6"/>
         <v>26.922699999999999</v>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
         <v>50.03</v>
       </c>
       <c r="D96" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E96">
         <v>2.2557999999999998</v>
@@ -2909,7 +2909,7 @@
         <v>7.2332999999999998</v>
       </c>
       <c r="G96">
-        <f>F96-E96</f>
+        <f t="shared" si="6"/>
         <v>4.9775</v>
       </c>
     </row>
@@ -2924,7 +2924,7 @@
         <v>50.03</v>
       </c>
       <c r="D97" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E97">
         <v>2.2364999999999999</v>
@@ -2933,7 +2933,7 @@
         <v>2.8180000000000001</v>
       </c>
       <c r="G97">
-        <f>F97-E97</f>
+        <f t="shared" si="6"/>
         <v>0.58150000000000013</v>
       </c>
     </row>
@@ -2948,7 +2948,7 @@
         <v>50.03</v>
       </c>
       <c r="D98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E98">
         <v>2.2368000000000001</v>
@@ -2957,7 +2957,7 @@
         <v>2.4218000000000002</v>
       </c>
       <c r="G98">
-        <f>F98-E98</f>
+        <f t="shared" si="6"/>
         <v>0.18500000000000005</v>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
         <v>15.76</v>
       </c>
       <c r="G99">
-        <f>F99-E99</f>
+        <f t="shared" si="6"/>
         <v>3.7099999999999991</v>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
         <v>50.05</v>
       </c>
       <c r="D100" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E100">
         <v>1.2595000000000001</v>
@@ -3005,7 +3005,7 @@
         <v>1.8945000000000001</v>
       </c>
       <c r="G100">
-        <f>F100-E100</f>
+        <f t="shared" si="6"/>
         <v>0.63500000000000001</v>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
         <v>10.7417</v>
       </c>
       <c r="G101">
-        <f>F101-E101</f>
+        <f t="shared" si="6"/>
         <v>9.4780999999999995</v>
       </c>
     </row>
@@ -3044,7 +3044,7 @@
         <v>50.05</v>
       </c>
       <c r="D102" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E102">
         <v>2.1850999999999998</v>
@@ -3053,7 +3053,7 @@
         <v>27.6266</v>
       </c>
       <c r="G102">
-        <f>F102-E102</f>
+        <f t="shared" si="6"/>
         <v>25.441500000000001</v>
       </c>
     </row>
@@ -3068,7 +3068,7 @@
         <v>50.05</v>
       </c>
       <c r="D103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E103">
         <v>2.1972999999999998</v>
@@ -3077,7 +3077,7 @@
         <v>11.6435</v>
       </c>
       <c r="G103">
-        <f>F103-E103</f>
+        <f t="shared" si="6"/>
         <v>9.4461999999999993</v>
       </c>
     </row>
@@ -3092,7 +3092,7 @@
         <v>50.05</v>
       </c>
       <c r="D104" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E104">
         <v>2.2465999999999999</v>
@@ -3101,7 +3101,7 @@
         <v>2.5966999999999998</v>
       </c>
       <c r="G104">
-        <f>F104-E104</f>
+        <f t="shared" si="6"/>
         <v>0.35009999999999986</v>
       </c>
     </row>
@@ -3116,7 +3116,7 @@
         <v>50.05</v>
       </c>
       <c r="D105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E105">
         <v>1.2765</v>
@@ -3125,7 +3125,7 @@
         <v>1.6495</v>
       </c>
       <c r="G105">
-        <f>F105-E105</f>
+        <f t="shared" si="6"/>
         <v>0.373</v>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
         <v>15.92</v>
       </c>
       <c r="G106">
-        <f>F106-E106</f>
+        <f t="shared" si="6"/>
         <v>3.7899999999999991</v>
       </c>
     </row>
@@ -3164,7 +3164,7 @@
         <v>50</v>
       </c>
       <c r="D107" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E107">
         <v>2.2492000000000001</v>
@@ -3173,7 +3173,7 @@
         <v>2.5367999999999999</v>
       </c>
       <c r="G107">
-        <f>F107-E107</f>
+        <f t="shared" si="6"/>
         <v>0.28759999999999986</v>
       </c>
     </row>
@@ -3197,7 +3197,7 @@
         <v>2.5648</v>
       </c>
       <c r="G108">
-        <f>F108-E108</f>
+        <f t="shared" si="6"/>
         <v>0.38759999999999994</v>
       </c>
     </row>
@@ -3212,7 +3212,7 @@
         <v>50</v>
       </c>
       <c r="D109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E109">
         <v>2.1713</v>
@@ -3221,7 +3221,7 @@
         <v>5.0747</v>
       </c>
       <c r="G109">
-        <f>F109-E109</f>
+        <f t="shared" si="6"/>
         <v>2.9034</v>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
         <v>50</v>
       </c>
       <c r="D110" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E110">
         <v>2.1688000000000001</v>
@@ -3245,7 +3245,7 @@
         <v>11.0769</v>
       </c>
       <c r="G110">
-        <f t="shared" ref="G110:G141" si="5">F110-E110</f>
+        <f t="shared" ref="G110:G141" si="7">F110-E110</f>
         <v>8.908100000000001</v>
       </c>
     </row>
@@ -3260,7 +3260,7 @@
         <v>50</v>
       </c>
       <c r="D111" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E111">
         <v>2.1758000000000002</v>
@@ -3269,7 +3269,7 @@
         <v>14.8833</v>
       </c>
       <c r="G111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12.7075</v>
       </c>
     </row>
@@ -3284,7 +3284,7 @@
         <v>50</v>
       </c>
       <c r="D112" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E112">
         <v>2.1663000000000001</v>
@@ -3293,7 +3293,7 @@
         <v>4.9546999999999999</v>
       </c>
       <c r="G112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7883999999999998</v>
       </c>
     </row>
@@ -3317,7 +3317,7 @@
         <v>17.45</v>
       </c>
       <c r="G113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.4699999999999989</v>
       </c>
     </row>
@@ -3341,7 +3341,7 @@
         <v>20.84</v>
       </c>
       <c r="G114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.0399999999999991</v>
       </c>
     </row>
@@ -3365,7 +3365,7 @@
         <v>17.48</v>
       </c>
       <c r="G115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.67</v>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
         <v>29.3</v>
       </c>
       <c r="G116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12.510000000000002</v>
       </c>
     </row>
@@ -3404,7 +3404,7 @@
         <v>50.15</v>
       </c>
       <c r="D117" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E117">
         <v>2.1052</v>
@@ -3413,7 +3413,7 @@
         <v>2.5142000000000002</v>
       </c>
       <c r="G117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.40900000000000025</v>
       </c>
     </row>
@@ -3437,7 +3437,7 @@
         <v>2.6718000000000002</v>
       </c>
       <c r="G118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.54260000000000019</v>
       </c>
     </row>
@@ -3452,7 +3452,7 @@
         <v>50.15</v>
       </c>
       <c r="D119" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E119">
         <v>2.0525000000000002</v>
@@ -3461,7 +3461,7 @@
         <v>5.5564999999999998</v>
       </c>
       <c r="G119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.5039999999999996</v>
       </c>
     </row>
@@ -3476,7 +3476,7 @@
         <v>50.15</v>
       </c>
       <c r="D120" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E120">
         <v>2.1781000000000001</v>
@@ -3485,7 +3485,7 @@
         <v>11.896699999999999</v>
       </c>
       <c r="G120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.7185999999999986</v>
       </c>
     </row>
@@ -3500,7 +3500,7 @@
         <v>50.15</v>
       </c>
       <c r="D121" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E121">
         <v>2.1987999999999999</v>
@@ -3509,7 +3509,7 @@
         <v>14.0618</v>
       </c>
       <c r="G121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.863</v>
       </c>
     </row>
@@ -3524,7 +3524,7 @@
         <v>50.15</v>
       </c>
       <c r="D122" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E122">
         <v>2.1379999999999999</v>
@@ -3533,7 +3533,7 @@
         <v>4.7112999999999996</v>
       </c>
       <c r="G122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.5732999999999997</v>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
         <v>20.2</v>
       </c>
       <c r="G123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1099999999999994</v>
       </c>
     </row>
@@ -3581,7 +3581,7 @@
         <v>26.87</v>
       </c>
       <c r="G124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.77</v>
       </c>
     </row>
@@ -3605,7 +3605,7 @@
         <v>21.92</v>
       </c>
       <c r="G125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.5700000000000021</v>
       </c>
     </row>
@@ -3620,7 +3620,7 @@
         <v>50.01</v>
       </c>
       <c r="D126" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E126">
         <v>2.0438000000000001</v>
@@ -3629,7 +3629,7 @@
         <v>2.3174000000000001</v>
       </c>
       <c r="G126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.27360000000000007</v>
       </c>
     </row>
@@ -3653,7 +3653,7 @@
         <v>2.3675999999999999</v>
       </c>
       <c r="G127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.29479999999999995</v>
       </c>
     </row>
@@ -3668,7 +3668,7 @@
         <v>50.01</v>
       </c>
       <c r="D128" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E128">
         <v>2.0419999999999998</v>
@@ -3677,7 +3677,7 @@
         <v>5.3821000000000003</v>
       </c>
       <c r="G128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.3401000000000005</v>
       </c>
     </row>
@@ -3692,7 +3692,7 @@
         <v>50.01</v>
       </c>
       <c r="D129" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E129">
         <v>2.1863999999999999</v>
@@ -3701,7 +3701,7 @@
         <v>10.737399999999999</v>
       </c>
       <c r="G129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.5509999999999984</v>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
         <v>50.01</v>
       </c>
       <c r="D130" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E130">
         <v>2.1063999999999998</v>
@@ -3725,7 +3725,7 @@
         <v>14.6777</v>
       </c>
       <c r="G130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12.571300000000001</v>
       </c>
     </row>
@@ -3740,7 +3740,7 @@
         <v>50.01</v>
       </c>
       <c r="D131" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E131">
         <v>2.2099000000000002</v>
@@ -3749,7 +3749,7 @@
         <v>5.0068000000000001</v>
       </c>
       <c r="G131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7968999999999999</v>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
         <v>20.07</v>
       </c>
       <c r="G132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1099999999999994</v>
       </c>
     </row>
@@ -3797,7 +3797,7 @@
         <v>23.71</v>
       </c>
       <c r="G133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.8900000000000006</v>
       </c>
       <c r="T133" s="14"/>
@@ -3824,7 +3824,7 @@
         <v>20.75</v>
       </c>
       <c r="G134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.6499999999999986</v>
       </c>
       <c r="O134" s="14"/>
@@ -3853,7 +3853,7 @@
         <v>20.65</v>
       </c>
       <c r="G135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.32</v>
       </c>
     </row>
@@ -3868,7 +3868,7 @@
         <v>50.08</v>
       </c>
       <c r="D136" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E136">
         <v>2.1415999999999999</v>
@@ -3877,7 +3877,7 @@
         <v>2.1415999999999999</v>
       </c>
       <c r="G136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
         <v>2.2313999999999998</v>
       </c>
       <c r="G137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -3916,7 +3916,7 @@
         <v>50.08</v>
       </c>
       <c r="D138" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E138">
         <v>2.1153</v>
@@ -3925,7 +3925,7 @@
         <v>2.1823000000000001</v>
       </c>
       <c r="G138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.7000000000000171E-2</v>
       </c>
     </row>
@@ -3940,7 +3940,7 @@
         <v>50.08</v>
       </c>
       <c r="D139" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E139">
         <v>2.1602000000000001</v>
@@ -3949,7 +3949,7 @@
         <v>2.8380999999999998</v>
       </c>
       <c r="G139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.67789999999999973</v>
       </c>
     </row>
@@ -3964,7 +3964,7 @@
         <v>50.08</v>
       </c>
       <c r="D140" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E140">
         <v>2.0619000000000001</v>
@@ -3973,7 +3973,7 @@
         <v>6.4965000000000002</v>
       </c>
       <c r="G140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.4345999999999997</v>
       </c>
     </row>
@@ -3988,7 +3988,7 @@
         <v>50.08</v>
       </c>
       <c r="D141" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E141">
         <v>2.1408</v>
@@ -3997,7 +3997,7 @@
         <v>10.620100000000001</v>
       </c>
       <c r="G141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.4793000000000003</v>
       </c>
     </row>
@@ -4021,7 +4021,7 @@
         <v>15.78</v>
       </c>
       <c r="G142">
-        <f t="shared" ref="G142:G164" si="6">F142-E142</f>
+        <f t="shared" ref="G142:G164" si="8">F142-E142</f>
         <v>3.9999999999999147E-2</v>
       </c>
     </row>
@@ -4045,7 +4045,7 @@
         <v>18.28</v>
       </c>
       <c r="G143">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.3500000000000014</v>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
         <v>48.56</v>
       </c>
       <c r="G144">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>32.430000000000007</v>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
         <v>16.3</v>
       </c>
       <c r="G145">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.0000000000000711E-2</v>
       </c>
     </row>
@@ -4108,7 +4108,7 @@
         <v>50.02</v>
       </c>
       <c r="D146" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E146">
         <v>2.1642000000000001</v>
@@ -4140,7 +4140,7 @@
         <v>2.1040999999999999</v>
       </c>
       <c r="G147">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.3999999999997392E-3</v>
       </c>
     </row>
@@ -4155,7 +4155,7 @@
         <v>50.02</v>
       </c>
       <c r="D148" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E148">
         <v>2.1762999999999999</v>
@@ -4164,7 +4164,7 @@
         <v>2.2688999999999999</v>
       </c>
       <c r="G148">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.2600000000000016E-2</v>
       </c>
     </row>
@@ -4179,7 +4179,7 @@
         <v>50.02</v>
       </c>
       <c r="D149" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E149">
         <v>2.1524999999999999</v>
@@ -4188,7 +4188,7 @@
         <v>2.8311000000000002</v>
       </c>
       <c r="G149">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.67860000000000031</v>
       </c>
     </row>
@@ -4203,7 +4203,7 @@
         <v>50.02</v>
       </c>
       <c r="D150" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E150">
         <v>2.1797</v>
@@ -4212,7 +4212,7 @@
         <v>5.7694999999999999</v>
       </c>
       <c r="G150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.5897999999999999</v>
       </c>
     </row>
@@ -4227,7 +4227,7 @@
         <v>50.02</v>
       </c>
       <c r="D151" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E151">
         <v>2.1941000000000002</v>
@@ -4236,7 +4236,7 @@
         <v>9.2599</v>
       </c>
       <c r="G151">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.0657999999999994</v>
       </c>
     </row>
@@ -4260,7 +4260,7 @@
         <v>15.81</v>
       </c>
       <c r="G152">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.0000000000001137E-2</v>
       </c>
     </row>
@@ -4284,7 +4284,7 @@
         <v>15.95</v>
       </c>
       <c r="G153">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.9999999999999147E-2</v>
       </c>
     </row>
@@ -4308,7 +4308,7 @@
         <v>48.84</v>
       </c>
       <c r="G154">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>32.760000000000005</v>
       </c>
     </row>
@@ -4332,7 +4332,7 @@
         <v>19.690000000000001</v>
       </c>
       <c r="G155">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.6500000000000021</v>
       </c>
     </row>
@@ -4347,7 +4347,7 @@
         <v>50.01</v>
       </c>
       <c r="D156" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E156">
         <v>2.2315</v>
@@ -4356,7 +4356,7 @@
         <v>2.3748999999999998</v>
       </c>
       <c r="G156">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.14339999999999975</v>
       </c>
     </row>
@@ -4380,7 +4380,7 @@
         <v>2.2532999999999999</v>
       </c>
       <c r="G157">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.7499999999999893E-2</v>
       </c>
     </row>
@@ -4395,7 +4395,7 @@
         <v>50.01</v>
       </c>
       <c r="D158" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E158">
         <v>2.1413000000000002</v>
@@ -4404,7 +4404,7 @@
         <v>2.4247999999999998</v>
       </c>
       <c r="G158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.28349999999999964</v>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
         <v>50.01</v>
       </c>
       <c r="D159" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E159">
         <v>2.2054</v>
@@ -4428,7 +4428,7 @@
         <v>3.3437000000000001</v>
       </c>
       <c r="G159">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1383000000000001</v>
       </c>
     </row>
@@ -4443,7 +4443,7 @@
         <v>50.01</v>
       </c>
       <c r="D160" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E160">
         <v>2.1722000000000001</v>
@@ -4452,7 +4452,7 @@
         <v>5.9775999999999998</v>
       </c>
       <c r="G160">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.8053999999999997</v>
       </c>
       <c r="X160" s="14"/>
@@ -4469,7 +4469,7 @@
         <v>50.01</v>
       </c>
       <c r="D161" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E161">
         <v>2.1059999999999999</v>
@@ -4478,7 +4478,7 @@
         <v>9.5892999999999997</v>
       </c>
       <c r="G161">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.4832999999999998</v>
       </c>
     </row>
@@ -4502,7 +4502,7 @@
         <v>15.93</v>
       </c>
       <c r="G162">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.75999999999999979</v>
       </c>
     </row>
@@ -4526,7 +4526,7 @@
         <v>20.09</v>
       </c>
       <c r="G163">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.8699999999999992</v>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
         <v>47.02</v>
       </c>
       <c r="G164">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.730000000000004</v>
       </c>
     </row>
@@ -4565,7 +4565,7 @@
         <v>100.15</v>
       </c>
       <c r="D165" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E165">
         <v>2.1027</v>
@@ -4574,7 +4574,7 @@
         <v>5.1978999999999997</v>
       </c>
       <c r="G165">
-        <f t="shared" ref="G165:G175" si="7">E165</f>
+        <f t="shared" ref="G165:G175" si="9">E165</f>
         <v>2.1027</v>
       </c>
     </row>
@@ -4598,7 +4598,7 @@
         <v>10.6663</v>
       </c>
       <c r="G166">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1065999999999998</v>
       </c>
     </row>
@@ -4613,7 +4613,7 @@
         <v>100.15</v>
       </c>
       <c r="D167" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E167">
         <v>2.1926999999999999</v>
@@ -4622,7 +4622,7 @@
         <v>36.496699999999997</v>
       </c>
       <c r="G167">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1926999999999999</v>
       </c>
     </row>
@@ -4637,7 +4637,7 @@
         <v>100.15</v>
       </c>
       <c r="D168" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E168">
         <v>2.1562000000000001</v>
@@ -4646,7 +4646,7 @@
         <v>22.6462</v>
       </c>
       <c r="G168">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1562000000000001</v>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
         <v>100.15</v>
       </c>
       <c r="D169" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E169">
         <v>2.1244999999999998</v>
@@ -4670,7 +4670,7 @@
         <v>6.7237999999999998</v>
       </c>
       <c r="G169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1244999999999998</v>
       </c>
     </row>
@@ -4685,7 +4685,7 @@
         <v>100.15</v>
       </c>
       <c r="D170" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E170">
         <v>2.2080000000000002</v>
@@ -4694,7 +4694,7 @@
         <v>3.6193</v>
       </c>
       <c r="G170">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.2080000000000002</v>
       </c>
     </row>
@@ -4718,7 +4718,7 @@
         <v>16.39</v>
       </c>
       <c r="G171">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.31</v>
       </c>
     </row>
@@ -4742,7 +4742,7 @@
         <v>16.47</v>
       </c>
       <c r="G172">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.33</v>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
         <v>16.739999999999998</v>
       </c>
       <c r="G173">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.46</v>
       </c>
     </row>
@@ -4790,7 +4790,7 @@
         <v>17.149999999999999</v>
       </c>
       <c r="G174">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.23</v>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
         <v>38.69</v>
       </c>
       <c r="G175">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.25</v>
       </c>
     </row>
@@ -4829,7 +4829,7 @@
         <v>100.63</v>
       </c>
       <c r="D176" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E176">
         <v>2.0733000000000001</v>
@@ -4838,7 +4838,7 @@
         <v>5.2640000000000002</v>
       </c>
       <c r="G176">
-        <f t="shared" ref="G176:G186" si="8">F176-E176</f>
+        <f t="shared" ref="G176:G186" si="10">F176-E176</f>
         <v>3.1907000000000001</v>
       </c>
     </row>
@@ -4862,7 +4862,7 @@
         <v>10.258699999999999</v>
       </c>
       <c r="G177">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.1560999999999986</v>
       </c>
       <c r="H177" s="9"/>
@@ -4878,7 +4878,7 @@
         <v>100.63</v>
       </c>
       <c r="D178" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E178">
         <v>2.1553</v>
@@ -4887,7 +4887,7 @@
         <v>35.517800000000001</v>
       </c>
       <c r="G178">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>33.362500000000004</v>
       </c>
     </row>
@@ -4902,7 +4902,7 @@
         <v>100.63</v>
       </c>
       <c r="D179" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E179">
         <v>2.1080000000000001</v>
@@ -4911,7 +4911,7 @@
         <v>24.1814</v>
       </c>
       <c r="G179">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22.073399999999999</v>
       </c>
     </row>
@@ -4926,7 +4926,7 @@
         <v>100.63</v>
       </c>
       <c r="D180" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E180">
         <v>2.1515</v>
@@ -4935,7 +4935,7 @@
         <v>6.6393000000000004</v>
       </c>
       <c r="G180">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.4878</v>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
         <v>100.63</v>
       </c>
       <c r="D181" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E181">
         <v>2.1297000000000001</v>
@@ -4959,7 +4959,7 @@
         <v>3.5952999999999999</v>
       </c>
       <c r="G181">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.4655999999999998</v>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
         <v>17.29</v>
       </c>
       <c r="G182">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9499999999999993</v>
       </c>
       <c r="N182" s="14"/>
@@ -5013,7 +5013,7 @@
         <v>17.84</v>
       </c>
       <c r="G183">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.5199999999999996</v>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
         <v>17.43</v>
       </c>
       <c r="G184">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.1099999999999994</v>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
         <v>17.45</v>
       </c>
       <c r="G185">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.129999999999999</v>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
         <v>37.6</v>
       </c>
       <c r="G186">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22.26</v>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
         <v>81.884099999999989</v>
       </c>
       <c r="D187" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E187">
         <v>2.1646999999999998</v>
@@ -5135,7 +5135,7 @@
         <v>11.987500000000001</v>
       </c>
       <c r="G188">
-        <f t="shared" ref="G188:G202" si="9">F188-E188</f>
+        <f t="shared" ref="G188:G202" si="11">F188-E188</f>
         <v>9.8474000000000004</v>
       </c>
     </row>
@@ -5150,7 +5150,7 @@
         <v>81.884100000000004</v>
       </c>
       <c r="D189" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E189">
         <v>2.1168</v>
@@ -5159,7 +5159,7 @@
         <v>37.1128</v>
       </c>
       <c r="G189">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>34.996000000000002</v>
       </c>
     </row>
@@ -5174,7 +5174,7 @@
         <v>81.884100000000004</v>
       </c>
       <c r="D190" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E190">
         <v>2.1760000000000002</v>
@@ -5183,7 +5183,7 @@
         <v>21.0595</v>
       </c>
       <c r="G190">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>18.883499999999998</v>
       </c>
     </row>
@@ -5198,7 +5198,7 @@
         <v>81.884100000000004</v>
       </c>
       <c r="D191" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E191">
         <v>2.1600999999999999</v>
@@ -5207,7 +5207,7 @@
         <v>6.0997000000000003</v>
       </c>
       <c r="G191">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.9396000000000004</v>
       </c>
       <c r="H191" s="9"/>
@@ -5230,7 +5230,7 @@
         <v>81.884100000000004</v>
       </c>
       <c r="D192" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E192">
         <v>2.1196000000000002</v>
@@ -5239,7 +5239,7 @@
         <v>3.3976999999999999</v>
       </c>
       <c r="G192">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.2780999999999998</v>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="G194">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.3999999999999986</v>
       </c>
     </row>
@@ -5311,7 +5311,7 @@
         <v>16.34</v>
       </c>
       <c r="G195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.3500000000000014</v>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="G196">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.36000000000000298</v>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
         <v>17.28</v>
       </c>
       <c r="G197">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.83999999999999986</v>
       </c>
     </row>
@@ -5383,7 +5383,7 @@
         <v>15.87</v>
       </c>
       <c r="G198">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1.2000000000000011</v>
       </c>
       <c r="H198" s="9"/>
@@ -5408,7 +5408,7 @@
         <v>16.239999999999998</v>
       </c>
       <c r="G199">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.66000000000000014</v>
       </c>
     </row>
@@ -5432,7 +5432,7 @@
         <v>20.95</v>
       </c>
       <c r="G200">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.7399999999999984</v>
       </c>
     </row>
@@ -5456,7 +5456,7 @@
         <v>16.64</v>
       </c>
       <c r="G201">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.41999999999999815</v>
       </c>
     </row>
@@ -5480,7 +5480,7 @@
         <v>31.2</v>
       </c>
       <c r="G202">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>13.969999999999999</v>
       </c>
     </row>
@@ -5730,42 +5730,6 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="K205:L205"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="X34:Z34"/>
-    <mergeCell ref="X160:Y160"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="O227:Q227"/>
-    <mergeCell ref="P239:Q239"/>
-    <mergeCell ref="J212:L212"/>
-    <mergeCell ref="O212:Q212"/>
-    <mergeCell ref="K224:L224"/>
-    <mergeCell ref="A290:C290"/>
-    <mergeCell ref="E290:G290"/>
-    <mergeCell ref="J290:L290"/>
-    <mergeCell ref="O290:Q290"/>
-    <mergeCell ref="O259:Q259"/>
-    <mergeCell ref="P271:Q271"/>
-    <mergeCell ref="K272:L272"/>
-    <mergeCell ref="J274:L274"/>
-    <mergeCell ref="O274:Q274"/>
-    <mergeCell ref="J259:L259"/>
-    <mergeCell ref="P286:Q286"/>
-    <mergeCell ref="A322:C322"/>
-    <mergeCell ref="E322:G322"/>
-    <mergeCell ref="J322:L322"/>
-    <mergeCell ref="O322:Q322"/>
-    <mergeCell ref="P302:Q302"/>
-    <mergeCell ref="F303:G303"/>
-    <mergeCell ref="K303:L303"/>
-    <mergeCell ref="A306:C306"/>
-    <mergeCell ref="E306:G306"/>
-    <mergeCell ref="J306:L306"/>
-    <mergeCell ref="O306:Q306"/>
-    <mergeCell ref="P318:Q318"/>
     <mergeCell ref="P210:Q210"/>
     <mergeCell ref="O191:Q191"/>
     <mergeCell ref="F335:G335"/>
@@ -5780,6 +5744,42 @@
     <mergeCell ref="O242:Q242"/>
     <mergeCell ref="P225:Q225"/>
     <mergeCell ref="J227:L227"/>
+    <mergeCell ref="A322:C322"/>
+    <mergeCell ref="E322:G322"/>
+    <mergeCell ref="J322:L322"/>
+    <mergeCell ref="O322:Q322"/>
+    <mergeCell ref="P302:Q302"/>
+    <mergeCell ref="F303:G303"/>
+    <mergeCell ref="K303:L303"/>
+    <mergeCell ref="A306:C306"/>
+    <mergeCell ref="E306:G306"/>
+    <mergeCell ref="J306:L306"/>
+    <mergeCell ref="O306:Q306"/>
+    <mergeCell ref="P318:Q318"/>
+    <mergeCell ref="A290:C290"/>
+    <mergeCell ref="E290:G290"/>
+    <mergeCell ref="J290:L290"/>
+    <mergeCell ref="O290:Q290"/>
+    <mergeCell ref="O259:Q259"/>
+    <mergeCell ref="P271:Q271"/>
+    <mergeCell ref="K272:L272"/>
+    <mergeCell ref="J274:L274"/>
+    <mergeCell ref="O274:Q274"/>
+    <mergeCell ref="J259:L259"/>
+    <mergeCell ref="P286:Q286"/>
+    <mergeCell ref="O227:Q227"/>
+    <mergeCell ref="P239:Q239"/>
+    <mergeCell ref="J212:L212"/>
+    <mergeCell ref="O212:Q212"/>
+    <mergeCell ref="K224:L224"/>
+    <mergeCell ref="K205:L205"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="X34:Z34"/>
+    <mergeCell ref="X160:Y160"/>
+    <mergeCell ref="S34:U34"/>
     <mergeCell ref="X187:Y187"/>
     <mergeCell ref="T133:U133"/>
     <mergeCell ref="O134:P134"/>

</xml_diff>